<commit_message>
Atualização do codigo, comentarios e estrutura do arquivo tabela.py. Adicionando o arquivo de dividendos.
</commit_message>
<xml_diff>
--- a/historico_dividendos.xlsx
+++ b/historico_dividendos.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Projeto_Financas_ativos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDEBD0C5-1755-43F5-B8DB-D62BE7A606E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF04648-397E-4E20-B167-B201A9ACAB57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="df_dividendos" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">df_dividendos!$A$1:$C$193</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -445,8 +448,8 @@
   </sheetPr>
   <dimension ref="A1:E193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
-      <selection activeCell="F181" sqref="F181"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B115" sqref="B115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,7 +1084,7 @@
         <v>45505</v>
       </c>
       <c r="C57" s="2">
-        <v>0.9</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1092,7 +1095,7 @@
         <v>45536</v>
       </c>
       <c r="C58" s="2">
-        <v>0.9</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1103,7 +1106,7 @@
         <v>45566</v>
       </c>
       <c r="C59" s="2">
-        <v>0.9</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1136,7 +1139,7 @@
         <v>45658</v>
       </c>
       <c r="C62" s="2">
-        <v>0.9</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1147,7 +1150,7 @@
         <v>45689</v>
       </c>
       <c r="C63" s="2">
-        <v>0.9</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1158,7 +1161,7 @@
         <v>45717</v>
       </c>
       <c r="C64" s="2">
-        <v>0.9</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1180,7 +1183,7 @@
         <v>45292</v>
       </c>
       <c r="C66" s="2">
-        <v>0.9</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1191,7 +1194,7 @@
         <v>45323</v>
       </c>
       <c r="C67" s="2">
-        <v>0.93</v>
+        <v>9.2999999999999999E-2</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1202,7 +1205,7 @@
         <v>45352</v>
       </c>
       <c r="C68" s="2">
-        <v>0.93</v>
+        <v>9.2999999999999999E-2</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1213,7 +1216,7 @@
         <v>45383</v>
       </c>
       <c r="C69" s="2">
-        <v>0.94</v>
+        <v>9.4E-2</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -1224,7 +1227,7 @@
         <v>45413</v>
       </c>
       <c r="C70" s="2">
-        <v>0.91</v>
+        <v>9.0999999999999998E-2</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -1235,7 +1238,7 @@
         <v>45444</v>
       </c>
       <c r="C71" s="2">
-        <v>0.91</v>
+        <v>9.0999999999999998E-2</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -1246,7 +1249,7 @@
         <v>45474</v>
       </c>
       <c r="C72" s="2">
-        <v>0.89</v>
+        <v>8.8999999999999996E-2</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -1257,7 +1260,7 @@
         <v>45505</v>
       </c>
       <c r="C73" s="2">
-        <v>0.89</v>
+        <v>8.8999999999999996E-2</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -1268,7 +1271,7 @@
         <v>45536</v>
       </c>
       <c r="C74" s="2">
-        <v>0.89</v>
+        <v>8.8999999999999996E-2</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -1279,7 +1282,7 @@
         <v>45566</v>
       </c>
       <c r="C75" s="2">
-        <v>0.91</v>
+        <v>9.0999999999999998E-2</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -1290,7 +1293,7 @@
         <v>45597</v>
       </c>
       <c r="C76" s="2">
-        <v>0.89</v>
+        <v>8.8999999999999996E-2</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -1301,7 +1304,7 @@
         <v>45627</v>
       </c>
       <c r="C77" s="2">
-        <v>0.89</v>
+        <v>8.8999999999999996E-2</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -1312,7 +1315,7 @@
         <v>45658</v>
       </c>
       <c r="C78" s="2">
-        <v>0.82</v>
+        <v>8.2000000000000003E-2</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -1323,7 +1326,7 @@
         <v>45689</v>
       </c>
       <c r="C79" s="2">
-        <v>0.9</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -1334,7 +1337,7 @@
         <v>45717</v>
       </c>
       <c r="C80" s="2">
-        <v>0.88</v>
+        <v>8.7999999999999995E-2</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -1345,7 +1348,7 @@
         <v>45748</v>
       </c>
       <c r="C81" s="2">
-        <v>0.92</v>
+        <v>9.1999999999999998E-2</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -2581,6 +2584,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C193" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>